<commit_message>
adding jsons for  5-16
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_5_9_12.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/envelope_5_9_12.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="14" documentId="8_{A5E81FF3-345E-4C39-B55F-73DF142E220B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85F5D22C-0A40-9A44-A6B7-0D4359521DDF}"/>
   <bookViews>
-    <workbookView xWindow="-37260" yWindow="2000" windowWidth="36320" windowHeight="18140" firstSheet="1" activeTab="2" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="1240" yWindow="680" windowWidth="36320" windowHeight="16640" firstSheet="1" activeTab="2" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -14381,10 +14381,10 @@
   <dimension ref="A1:BF128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X6" sqref="X6"/>
+      <selection pane="bottomRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>